<commit_message>
Update cross reference code
</commit_message>
<xml_diff>
--- a/input/ref/cross_reference.xlsx
+++ b/input/ref/cross_reference.xlsx
@@ -10,7 +10,11 @@
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
     <sheet name="Client_Project" sheetId="2" r:id="rId2"/>
     <sheet name="Job" sheetId="3" r:id="rId3"/>
+    <sheet name="Raw Records" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Raw Records'!$B$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
   <si>
     <t>Project Name</t>
   </si>
@@ -47,12 +51,6 @@
     <t>Assumption</t>
   </si>
   <si>
-    <t>WSCCWC (Premium Rate Setting)</t>
-  </si>
-  <si>
-    <t>WSCCWC (Accounting Valuation)</t>
-  </si>
-  <si>
     <t>681540</t>
   </si>
   <si>
@@ -90,13 +88,178 @@
   </si>
   <si>
     <t>ZZZ (Internal Training)</t>
+  </si>
+  <si>
+    <t>ZZZ (Vacation)</t>
+  </si>
+  <si>
+    <t>ZZZ (Sick)</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>686502</t>
+  </si>
+  <si>
+    <t>NWTWCBWC WSCC of NWT and Nunavut WC - F
+ [Accounting Valuation]</t>
+  </si>
+  <si>
+    <t>NWTWCBOPEB WSCC of NWT and Nunavut OPEB -
+ [Accounting Valuation]</t>
+  </si>
+  <si>
+    <t>PPEWC Prov. of PEI WC - Fee for Serv
+ [Accounting Valuation]</t>
+  </si>
+  <si>
+    <t>PEIWCBWC Workers Comp. Board of PEI WC
+ [Premium rate setting]</t>
+  </si>
+  <si>
+    <t>NWTWCBWC WSCC of NWT and Nunavut WC - F
+ [Premium rate setting]</t>
+  </si>
+  <si>
+    <t>NBWHSCWC WorkSafe NB WC - Fee for Servi
+ [Accounting Valuation]</t>
+  </si>
+  <si>
+    <t>NBWHSCWC WorkSafe NB WC - Fee for Servi
+ [Special Val./Analysis/ALM/Nego]</t>
+  </si>
+  <si>
+    <t>PNBDFOC PNB Dept Fin Other Consulting
+ [Other Consulting]</t>
+  </si>
+  <si>
+    <t>PNLWC Prov. of NL WC - Fee for Servi
+ [Special Val./Analysis/ALM/Nego]</t>
+  </si>
+  <si>
+    <t>10001004</t>
+  </si>
+  <si>
+    <t>10001005</t>
+  </si>
+  <si>
+    <t>10003510</t>
+  </si>
+  <si>
+    <t>NWTWCBWC WSCC of NWT and Nunavut WC - F
+ [Client Management]</t>
+  </si>
+  <si>
+    <t>10001018</t>
+  </si>
+  <si>
+    <t>10000705</t>
+  </si>
+  <si>
+    <t>10000920</t>
+  </si>
+  <si>
+    <t>10000906</t>
+  </si>
+  <si>
+    <t>10000914</t>
+  </si>
+  <si>
+    <t>10001019</t>
+  </si>
+  <si>
+    <t>10001001</t>
+  </si>
+  <si>
+    <t>NBWHSCWC WorkSafe NB WC - Fee for Servi
+ [Premium Rate Setting]</t>
+  </si>
+  <si>
+    <t>WSNB-WC</t>
+  </si>
+  <si>
+    <t>WSCC-OPEB</t>
+  </si>
+  <si>
+    <t>WSCC-WC</t>
+  </si>
+  <si>
+    <t>PEIWCB-WC</t>
+  </si>
+  <si>
+    <t>PNB-DoF</t>
+  </si>
+  <si>
+    <t>PNB-Drug</t>
+  </si>
+  <si>
+    <t>PNL-WC</t>
+  </si>
+  <si>
+    <t>PPE-WC</t>
+  </si>
+  <si>
+    <t>Premium Rate Setting</t>
+  </si>
+  <si>
+    <t>Accounting Valuation</t>
+  </si>
+  <si>
+    <t>Special Analysis</t>
+  </si>
+  <si>
+    <t>Client Management</t>
+  </si>
+  <si>
+    <t>PNBPDP Province of NB - Prescription
+ [Premium rate setting]</t>
+  </si>
+  <si>
+    <t>Other Consulting</t>
+  </si>
+  <si>
+    <t>WSNB-WC (Accounting Valuation)</t>
+  </si>
+  <si>
+    <t>WSNB-WC (Premium Rate Setting)</t>
+  </si>
+  <si>
+    <t>WSNB-WC (Special Analysis)</t>
+  </si>
+  <si>
+    <t>WSCC-OPEB (Accounting Valuation)</t>
+  </si>
+  <si>
+    <t>WSCC-WC (Accounting Valuation)</t>
+  </si>
+  <si>
+    <t>WSCC-WC (Client Management)</t>
+  </si>
+  <si>
+    <t>WSCC-WC (Premium Rate Setting)</t>
+  </si>
+  <si>
+    <t>PEIWCB-WC (Premium Rate Setting)</t>
+  </si>
+  <si>
+    <t>PNB-DoF (Other Consulting)</t>
+  </si>
+  <si>
+    <t>PNB-Drug (Premium Rate Setting)</t>
+  </si>
+  <si>
+    <t>PNL-WC (Special Analysis)</t>
+  </si>
+  <si>
+    <t>PPE-WC (Accounting Valuation)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +282,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0F0F0F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -128,7 +298,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,15 +306,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +668,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D8"/>
+  <dimension ref="B3:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,51 +679,52 @@
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="str">
         <f>B3&amp;"Number"</f>
         <v>ClientProjectNumber</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="2">
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -527,10 +732,10 @@
         <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -538,10 +743,142 @@
         <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2">
-        <v>106</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -551,10 +888,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C7"/>
+  <dimension ref="B3:C8"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +903,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="str">
         <f>B3&amp;"Number"</f>
@@ -578,7 +915,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -586,7 +923,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -594,7 +931,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -602,8 +939,260 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="75" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>C2&amp;" ("&amp;D2&amp;")"</f>
+        <v>WSNB-WC (Accounting Valuation)</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="4" t="str">
+        <f t="shared" ref="E3:E13" si="0">C3&amp;" ("&amp;D3&amp;")"</f>
+        <v>WSNB-WC (Premium Rate Setting)</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>WSNB-WC (Special Analysis)</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>WSCC-OPEB (Accounting Valuation)</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>WSCC-WC (Accounting Valuation)</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>WSCC-WC (Client Management)</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>WSCC-WC (Premium Rate Setting)</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PEIWCB-WC (Premium Rate Setting)</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PNB-DoF (Other Consulting)</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PNB-Drug (Premium Rate Setting)</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PNL-WC (Special Analysis)</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PPE-WC (Accounting Valuation)</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New project time codes
</commit_message>
<xml_diff>
--- a/input/ref/cross_reference.xlsx
+++ b/input/ref/cross_reference.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
   <si>
     <t>Project Name</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>PPE-WC (Accounting Valuation)</t>
+  </si>
+  <si>
+    <t>ZZZ (Marketing Specific Prospect)</t>
   </si>
 </sst>
 </file>
@@ -298,7 +301,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -306,26 +309,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -335,9 +323,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -345,9 +330,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -668,16 +650,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D20"/>
+  <dimension ref="B3:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -751,32 +733,32 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -784,10 +766,10 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -795,10 +777,10 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -806,10 +788,10 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
@@ -817,10 +799,10 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -828,10 +810,10 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -839,10 +821,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -850,10 +832,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
@@ -861,10 +843,10 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -872,12 +854,23 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D21" s="2">
         <v>0</v>
       </c>
     </row>
@@ -960,7 +953,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,13 +968,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="4" t="str">
@@ -993,13 +986,13 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E3" s="4" t="str">
@@ -1011,13 +1004,13 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="4" t="str">
@@ -1029,13 +1022,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="4" t="str">
@@ -1047,13 +1040,13 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E6" s="4" t="str">
@@ -1065,133 +1058,133 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>57</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>WSCC-WC (Client Management)</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>WSCC-WC (Premium Rate Setting)</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>PEIWCB-WC (Premium Rate Setting)</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>PNB-DoF (Other Consulting)</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>PNB-Drug (Premium Rate Setting)</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>PNL-WC (Special Analysis)</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>PPE-WC (Accounting Valuation)</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
   </sheetData>

</xml_diff>